<commit_message>
lab 4 add check list
</commit_message>
<xml_diff>
--- a/lab4/test_scenario.xlsx
+++ b/lab4/test_scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaptot/Desktop/testing_bsu/lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7376A047-832D-C24C-9B11-81DB59C4F6D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7883C2BB-86B7-F142-ACC9-A8E7CE6B47D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C6D04D7B-6147-CD46-82BB-E215CE389BDE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{C6D04D7B-6147-CD46-82BB-E215CE389BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>№</t>
   </si>
@@ -100,6 +100,38 @@
   <si>
     <t>1. Заполнить все поля
 2. Нажать кнопку "Отмена"</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта при незаполненом поле "Сокращенное название"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле "Название", например значением "я люблю сокращать названия"
+2. Нажать кнопку сохранить</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта при заполнении поля "Название" невалидным значением</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле "Название" невалидным значением, например, "Проеееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееект 1"
+2. Заполнить поле "Сокращенное название" допустимым значением, например "Сокращение 1"
+3. Нажать кнопку сохранить</t>
+  </si>
+  <si>
+    <t>отображение алерта об незаполненном обязательно поле "Сокращенное название"</t>
+  </si>
+  <si>
+    <t>отображение алерта об неверном заполнении обязательного поля  "Название"</t>
+  </si>
+  <si>
+    <t>Попытка создания проекта при заполнении поля "Сокращенное название" невалидным значением</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле "Сокращенное название" невалидным значением, например, "Проеееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееееект 1"
+2. Заполнить поле "Сокращенное название" допустимым значением, например "Сокращение 1"
+3. Нажать кнопку сохранить</t>
+  </si>
+  <si>
+    <t>отображение алерта об неверном заполнении обязательного поля  "Сокращенное название"</t>
   </si>
 </sst>
 </file>
@@ -107,12 +139,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,8 +166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -141,15 +179,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -158,11 +197,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8F50FC-C760-3F4B-9BC3-BFBC38C54D35}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +529,7 @@
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.83203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -518,7 +561,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -538,7 +581,7 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
@@ -556,7 +599,7 @@
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
@@ -574,7 +617,7 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
@@ -592,7 +635,7 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
@@ -603,14 +646,59 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="3"/>
+    <row r="7" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F10" s="3"/>
@@ -683,7 +771,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C2:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>